<commit_message>
Updated daily notes and Table 1, still missing info
</commit_message>
<xml_diff>
--- a/Data_fullset.xlsx
+++ b/Data_fullset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Pulmonary Edema</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Peripheral Edema</t>
   </si>
   <si>
-    <t>No History Found</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -40,6 +37,39 @@
   </si>
   <si>
     <t>Addendums (approx)</t>
+  </si>
+  <si>
+    <t>Of pts with all info:</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>No Exam Found</t>
+  </si>
+  <si>
+    <t># of pts</t>
+  </si>
+  <si>
+    <t>Percent of all info pts</t>
+  </si>
+  <si>
+    <t>REVISED: NEONATES REMOVED.</t>
+  </si>
+  <si>
+    <t>#patients</t>
+  </si>
+  <si>
+    <t>No Exam</t>
+  </si>
+  <si>
+    <t>Percent total</t>
+  </si>
+  <si>
+    <t>All Info</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -379,30 +409,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
       <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -417,7 +451,7 @@
         <v>0.48824071939128427</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -432,7 +466,7 @@
         <v>7.7280762431788483E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -447,7 +481,7 @@
         <v>5.8104680654830529E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -462,7 +496,7 @@
         <v>7.3168857120897698E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -477,7 +511,7 @@
         <v>3.2203520098378298E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -492,7 +526,7 @@
         <v>5.2647759588040893E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-1</v>
       </c>
@@ -507,7 +541,7 @@
         <v>2.9282914456997926E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-1</v>
       </c>
@@ -522,7 +556,7 @@
         <v>1.9983091230497273E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -537,9 +571,9 @@
         <v>2.782261163630774E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>5377</v>
@@ -549,9 +583,9 @@
         <v>0.20663284912766122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
         <f>SUM(C2:C11)</f>
@@ -562,30 +596,416 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
         <f>(C4+C7+C8+C9+C10+C11)/C12</f>
         <v>0.32910614095765123</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="F15" s="1">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
         <f>(C2+C3+C5+C6)/C12</f>
         <v>0.67089385904234877</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
-        <v>2301</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12705</v>
+      </c>
+      <c r="D19">
+        <f>C19/C23</f>
+        <v>0.72774659182036894</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D20">
+        <f>C20/C23</f>
+        <v>0.11519074349868255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1904</v>
+      </c>
+      <c r="D21">
+        <f>C21/C23</f>
+        <v>0.10906174819566961</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>838</v>
+      </c>
+      <c r="D22">
+        <f>C22/C23</f>
+        <v>4.8000916485278954E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <f>SUM(C19:C22)</f>
+        <v>17458</v>
+      </c>
+      <c r="D23">
+        <f>SUM(D19:D22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>838</v>
+      </c>
+      <c r="D27">
+        <f>C27/C37</f>
+        <v>3.7120708748615727E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1751</v>
+      </c>
+      <c r="D28">
+        <f>C28/C37</f>
+        <v>7.7563676633444073E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>-1</v>
+      </c>
+      <c r="C29">
+        <v>96</v>
+      </c>
+      <c r="D29">
+        <f>C29/C37</f>
+        <v>4.2524916943521597E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>2009</v>
+      </c>
+      <c r="D30">
+        <f>C30/C37</f>
+        <v>8.89922480620155E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>11308</v>
+      </c>
+      <c r="D31">
+        <f>C31/C37</f>
+        <v>0.50090808416389809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>-1</v>
+      </c>
+      <c r="C32">
+        <v>1145</v>
+      </c>
+      <c r="D32">
+        <f>C32/C37</f>
+        <v>5.0719822812846066E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <f>C33/C37</f>
+        <v>2.3034330011074198E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-1</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>539</v>
+      </c>
+      <c r="D34">
+        <f>C34/C37</f>
+        <v>2.3875968992248062E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-1</v>
+      </c>
+      <c r="B35">
+        <v>-1</v>
+      </c>
+      <c r="C35">
+        <v>557</v>
+      </c>
+      <c r="D35">
+        <f>C35/C37</f>
+        <v>2.4673311184939092E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>4280</v>
+      </c>
+      <c r="D36">
+        <f>C36/C37</f>
+        <v>0.18959025470653379</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <f>SUM(C27:C36)</f>
+        <v>22575</v>
+      </c>
+      <c r="D37">
+        <f>SUM(D27:D36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <f>(C29+C32+C33+C34+C35+C36)/C37</f>
+        <v>0.29541528239202658</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <f>1-B39</f>
+        <v>0.70458471760797337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>838</v>
+      </c>
+      <c r="D43">
+        <f>C43/C47</f>
+        <v>5.2684521564189617E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>1751</v>
+      </c>
+      <c r="D44">
+        <f>C44/C47</f>
+        <v>0.11008424493901672</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>2009</v>
+      </c>
+      <c r="D45">
+        <f>C45/C47</f>
+        <v>0.1263045391676097</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>11308</v>
+      </c>
+      <c r="D46">
+        <f>C46/C47</f>
+        <v>0.71092669432918398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f>SUM(C43:C46)</f>
+        <v>15906</v>
+      </c>
+      <c r="D47">
+        <f>SUM(D43:D46)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>